<commit_message>
Results from February_11,_2021--17:28:40 run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2021-02-10.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2021-02-10.xlsx
@@ -911,16 +911,16 @@
         <v>22</v>
       </c>
       <c r="B9" s="2">
-        <v>44236</v>
+        <v>44237</v>
       </c>
       <c r="C9">
-        <v>147932</v>
+        <v>148475</v>
       </c>
       <c r="D9">
-        <v>2031</v>
+        <v>2044</v>
       </c>
       <c r="E9">
-        <v>3570</v>
+        <v>3586</v>
       </c>
       <c r="F9">
         <v>44</v>
@@ -929,7 +929,7 @@
         <v>2.96</v>
       </c>
       <c r="H9">
-        <v>2.57</v>
+        <v>2.55</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -938,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <v>120677</v>
+        <v>121163</v>
       </c>
       <c r="L9">
-        <v>1714</v>
+        <v>1723</v>
       </c>
       <c r="M9">
         <v>77789</v>
@@ -2079,11 +2079,32 @@
       <c r="A43" t="s">
         <v>56</v>
       </c>
+      <c r="B43" s="2">
+        <v>44237</v>
+      </c>
+      <c r="C43">
+        <v>112993</v>
+      </c>
+      <c r="D43">
+        <v>1791</v>
+      </c>
+      <c r="E43">
+        <v>973</v>
+      </c>
+      <c r="F43">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>0.86</v>
+      </c>
+      <c r="H43">
+        <v>0.5</v>
+      </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43">
         <v>11536</v>
@@ -2092,7 +2113,7 @@
         <v>0.68</v>
       </c>
       <c r="O43" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:15">

</xml_diff>